<commit_message>
add cites, add grundlagen and othello game infomation
</commit_message>
<xml_diff>
--- a/Paper/Bericht/Grafiken.xlsx
+++ b/Paper/Bericht/Grafiken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Semester5\T3000\othello\Paper\Bericht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9997A81B-65F3-419C-806E-59FA71EA38BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A24B0-63E1-491B-AF27-8EC4D9FAA0FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{E55107AA-2CE7-440E-BDEC-F1324765409F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="11">
   <si>
     <t>A</t>
   </si>
@@ -86,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +111,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -214,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -245,6 +269,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,15 +615,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7FF6C3-614F-470E-93E4-1B37645D0040}">
-  <dimension ref="D1:L9"/>
+  <dimension ref="D1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="4:12" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="4:45" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +648,80 @@
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -611,8 +737,41 @@
         <v>2</v>
       </c>
       <c r="L2" s="8"/>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="14"/>
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="14"/>
+      <c r="AK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
+      <c r="AP2" s="13"/>
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="13"/>
+      <c r="AS2" s="14"/>
     </row>
-    <row r="3" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D3" s="1">
         <v>2</v>
       </c>
@@ -632,8 +791,41 @@
       <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="17"/>
+      <c r="Z3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="17"/>
+      <c r="AK3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="17"/>
     </row>
-    <row r="4" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D4" s="1">
         <v>3</v>
       </c>
@@ -645,8 +837,41 @@
       <c r="J4" s="6"/>
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
+      <c r="O4" s="1">
+        <v>3</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="17"/>
+      <c r="Z4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="17"/>
+      <c r="AK4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
+      <c r="AQ4" s="16"/>
+      <c r="AR4" s="16"/>
+      <c r="AS4" s="17"/>
     </row>
-    <row r="5" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D5" s="1">
         <v>4</v>
       </c>
@@ -662,8 +887,53 @@
       <c r="J5" s="6"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
+      <c r="O5" s="1">
+        <v>4</v>
+      </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="17"/>
+      <c r="Z5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="17"/>
+      <c r="AK5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ5" s="16"/>
+      <c r="AR5" s="16"/>
+      <c r="AS5" s="17"/>
     </row>
-    <row r="6" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D6" s="1">
         <v>5</v>
       </c>
@@ -679,8 +949,57 @@
       <c r="J6" s="6"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
+      <c r="O6" s="1">
+        <v>5</v>
+      </c>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="18"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="17"/>
+      <c r="Z6" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="17"/>
+      <c r="AK6" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="16"/>
+      <c r="AO6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR6" s="16"/>
+      <c r="AS6" s="17"/>
     </row>
-    <row r="7" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D7" s="1">
         <v>6</v>
       </c>
@@ -692,8 +1011,41 @@
       <c r="J7" s="6"/>
       <c r="K7" s="4"/>
       <c r="L7" s="5"/>
+      <c r="O7" s="1">
+        <v>6</v>
+      </c>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="17"/>
+      <c r="Z7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="17"/>
+      <c r="AK7" s="1">
+        <v>6</v>
+      </c>
+      <c r="AL7" s="15"/>
+      <c r="AM7" s="16"/>
+      <c r="AN7" s="16"/>
+      <c r="AO7" s="16"/>
+      <c r="AP7" s="16"/>
+      <c r="AQ7" s="16"/>
+      <c r="AR7" s="16"/>
+      <c r="AS7" s="17"/>
     </row>
-    <row r="8" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="8" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D8" s="1">
         <v>7</v>
       </c>
@@ -713,8 +1065,41 @@
       <c r="L8" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="O8" s="1">
+        <v>7</v>
+      </c>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="17"/>
+      <c r="Z8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="17"/>
+      <c r="AK8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="16"/>
+      <c r="AN8" s="16"/>
+      <c r="AO8" s="16"/>
+      <c r="AP8" s="16"/>
+      <c r="AQ8" s="16"/>
+      <c r="AR8" s="16"/>
+      <c r="AS8" s="17"/>
     </row>
-    <row r="9" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="D9" s="1">
         <v>8</v>
       </c>
@@ -730,6 +1115,39 @@
         <v>2</v>
       </c>
       <c r="L9" s="11"/>
+      <c r="O9" s="1">
+        <v>8</v>
+      </c>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="17"/>
+      <c r="Z9" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="17"/>
+      <c r="AK9" s="1">
+        <v>8</v>
+      </c>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="16"/>
+      <c r="AN9" s="16"/>
+      <c r="AO9" s="16"/>
+      <c r="AP9" s="16"/>
+      <c r="AQ9" s="16"/>
+      <c r="AR9" s="16"/>
+      <c r="AS9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish section on Nijssen 07 Heuristic
</commit_message>
<xml_diff>
--- a/Paper/Bericht/Grafiken.xlsx
+++ b/Paper/Bericht/Grafiken.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Semester5\T3000\othello\Paper\Bericht\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A24B0-63E1-491B-AF27-8EC4D9FAA0FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{E55107AA-2CE7-440E-BDEC-F1324765409F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12168"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="11">
   <si>
     <t>A</t>
   </si>
@@ -69,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -607,21 +602,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7FF6C3-614F-470E-93E4-1B37645D0040}">
-  <dimension ref="D1:AS9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:AS20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="52.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="4:45" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="E1" s="1" t="s">
@@ -1149,8 +1144,214 @@
       <c r="AR9" s="16"/>
       <c r="AS9" s="17"/>
     </row>
+    <row r="12" spans="4:45" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:45" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D17" s="1">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D19" s="1">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.85">
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>